<commit_message>
Refactor Expert System and update dependencies
- Remove TensorFlow.js and related dependencies
- Add PapaParse and Chart.js for data processing and visualization
- Update package.json and package-lock.json with new dependencies
- Simplify ExpertSystem page by extracting component logic
- Update BottomNav with new icon and text for Expert System section
</commit_message>
<xml_diff>
--- a/public/filetest.xlsx
+++ b/public/filetest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8306D244-D734-480B-AABC-5DA269FB5059}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5712DA2D-F92A-4434-8660-146184324C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3396" activeTab="1" xr2:uid="{865F1972-1110-407E-98C8-8DE8E3094A15}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Refactor Processvideo component with improved error handling and workflow
- Remove ProgressIndicator and ErrorMessage components
- Add reset functionality for image processing
- Simplify loading and error states
- Implement file input reference for better file selection
- Update API interaction with more robust error handling
- Add button to restart image processing after completion
</commit_message>
<xml_diff>
--- a/public/filetest.xlsx
+++ b/public/filetest.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5712DA2D-F92A-4434-8660-146184324C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9225F39-C7B6-4E25-B744-AEE715E27E7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3396" activeTab="1" xr2:uid="{865F1972-1110-407E-98C8-8DE8E3094A15}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3396" xr2:uid="{865F1972-1110-407E-98C8-8DE8E3094A15}"/>
   </bookViews>
   <sheets>
-    <sheet name="Preguntas" sheetId="1" r:id="rId1"/>
-    <sheet name="Conocimiento" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -26,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>pregunta</t>
-  </si>
-  <si>
-    <t>escalabilidad</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>¿Se requiere alta escalabilidad?</t>
   </si>
   <si>
-    <t>despliegue_rapido</t>
-  </si>
-  <si>
     <t>¿Se necesita un despliegue rápido y frecuente de nuevas funcionalidades?</t>
   </si>
   <si>
@@ -70,33 +57,6 @@
     <t>¿Se requiere procesamiento asíncrono o en tiempo real de eventos?</t>
   </si>
   <si>
-    <t xml:space="preserve"> presupuesto_limitado</t>
-  </si>
-  <si>
-    <t>picos_demanda</t>
-  </si>
-  <si>
-    <t>separacion_responsabilidades</t>
-  </si>
-  <si>
-    <t>tolerancia_fallos</t>
-  </si>
-  <si>
-    <t>requisitos_cambiantes</t>
-  </si>
-  <si>
-    <t>minimizar_servidores</t>
-  </si>
-  <si>
-    <t>mantenibilidad</t>
-  </si>
-  <si>
-    <t>procesamiento_asincrono</t>
-  </si>
-  <si>
-    <t>respuesta</t>
-  </si>
-  <si>
     <t>Arquitectura Monolítica</t>
   </si>
   <si>
@@ -110,6 +70,9 @@
   </si>
   <si>
     <t>Arquitectura Event-Driven (Basada en Eventos)</t>
+  </si>
+  <si>
+    <t>Decisión</t>
   </si>
 </sst>
 </file>
@@ -463,114 +426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3E9F8B-FE1E-48C9-8270-B4219123A00B}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:E28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C5597A-5F7F-4E0D-9535-FC37BBE5E1F0}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,37 +448,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -653,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -688,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -723,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -755,10 +615,10 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -793,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>